<commit_message>
Added drops to fight
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d7be89ac2d74e3b/Documents/GitHub/RPG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{88A4C000-A471-49DD-BCDA-369CDE128E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B6CC2CA-4A70-4DD5-B97D-39510537FF47}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{88A4C000-A471-49DD-BCDA-369CDE128E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E47955B8-3B85-4D4B-904B-28B18BAF9758}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AFF9EEE-D23B-4E8B-9C8E-5BF4B0F735F6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Description</t>
   </si>
@@ -104,6 +104,21 @@
   </si>
   <si>
     <t>0-2</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Gem</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Guh</t>
+  </si>
+  <si>
+    <t>Shiny</t>
   </si>
 </sst>
 </file>
@@ -458,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FEC809A-A91F-4ACB-8EE8-79CADBAB716F}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,6 +592,40 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed Buttons and overall fight command.
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -476,7 +476,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>